<commit_message>
Testng Data Provider testing example
</commit_message>
<xml_diff>
--- a/DataDrivenTesting.xlsx
+++ b/DataDrivenTesting.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
-    <sheet name="Username&amp;Password" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
     <sheet name="Credentials" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>heat</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -393,14 +396,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -410,7 +449,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>